<commit_message>
update to final data version
</commit_message>
<xml_diff>
--- a/Results/Plot data/ipcc_ar6_figure_equity_perspectives.xlsx
+++ b/Results/Plot data/ipcc_ar6_figure_equity_perspectives.xlsx
@@ -24,7 +24,7 @@
     <t xml:space="preserve">Last update</t>
   </si>
   <si>
-    <t xml:space="preserve">2021-08-24 13:56:51</t>
+    <t xml:space="preserve">2021-09-24 11:16:54</t>
   </si>
   <si>
     <t xml:space="preserve">Code</t>
@@ -63,7 +63,7 @@
     <t xml:space="preserve">Historical cumulative emissions</t>
   </si>
   <si>
-    <t xml:space="preserve">1189 Gt CO2</t>
+    <t xml:space="preserve">1190 Gt CO2</t>
   </si>
   <si>
     <t xml:space="preserve">Asia and developing Pacific</t>
@@ -117,7 +117,7 @@
     <t xml:space="preserve">Cumulative CO2 of countries between 65 and 75yrs life expectancy (1970-2018)</t>
   </si>
   <si>
-    <t xml:space="preserve">604 Gt CO2</t>
+    <t xml:space="preserve">605 Gt CO2</t>
   </si>
   <si>
     <t xml:space="preserve">Cumulative CO2 of countries below 65yrs life expectancy (1970-2018)</t>
@@ -129,13 +129,13 @@
     <t xml:space="preserve">Territorial GHG, excl. LULUCF (2019)</t>
   </si>
   <si>
-    <t xml:space="preserve">50 Gt CO2eq</t>
+    <t xml:space="preserve">51 Gt CO2eq</t>
   </si>
   <si>
     <t xml:space="preserve">Territorial GHG, incl. LULUCF (2019)</t>
   </si>
   <si>
-    <t xml:space="preserve">57 Gt CO2eq</t>
+    <t xml:space="preserve">58 Gt CO2eq</t>
   </si>
 </sst>
 </file>
@@ -533,7 +533,7 @@
         <v>13</v>
       </c>
       <c r="B2" t="n">
-        <v>41176703545.0527</v>
+        <v>41241446843.9533</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -542,10 +542,10 @@
         <v>15</v>
       </c>
       <c r="E2" t="n">
-        <v>1188540811061.7</v>
+        <v>1189679505864.58</v>
       </c>
       <c r="F2" t="n">
-        <v>0.034644753601915</v>
+        <v>0.0346660143682829</v>
       </c>
       <c r="G2" t="s">
         <v>16</v>
@@ -556,7 +556,7 @@
         <v>17</v>
       </c>
       <c r="B3" t="n">
-        <v>326050102398.452</v>
+        <v>326712801404.424</v>
       </c>
       <c r="C3" t="s">
         <v>14</v>
@@ -565,10 +565,10 @@
         <v>15</v>
       </c>
       <c r="E3" t="n">
-        <v>1188540811061.7</v>
+        <v>1189679505864.58</v>
       </c>
       <c r="F3" t="n">
-        <v>0.274328066284235</v>
+        <v>0.274622534719542</v>
       </c>
       <c r="G3" t="s">
         <v>16</v>
@@ -579,7 +579,7 @@
         <v>18</v>
       </c>
       <c r="B4" t="n">
-        <v>598971855842.451</v>
+        <v>599201738199.917</v>
       </c>
       <c r="C4" t="s">
         <v>14</v>
@@ -588,10 +588,10 @@
         <v>15</v>
       </c>
       <c r="E4" t="n">
-        <v>1188540811061.7</v>
+        <v>1189679505864.58</v>
       </c>
       <c r="F4" t="n">
-        <v>0.503955649034384</v>
+        <v>0.503666521316138</v>
       </c>
       <c r="G4" t="s">
         <v>16</v>
@@ -602,7 +602,7 @@
         <v>19</v>
       </c>
       <c r="B5" t="n">
-        <v>114666190179.966</v>
+        <v>114687068188.585</v>
       </c>
       <c r="C5" t="s">
         <v>14</v>
@@ -611,10 +611,10 @@
         <v>15</v>
       </c>
       <c r="E5" t="n">
-        <v>1188540811061.7</v>
+        <v>1189679505864.58</v>
       </c>
       <c r="F5" t="n">
-        <v>0.0964764433099589</v>
+        <v>0.0964016507162051</v>
       </c>
       <c r="G5" t="s">
         <v>16</v>
@@ -625,7 +625,7 @@
         <v>20</v>
       </c>
       <c r="B6" t="n">
-        <v>57616809562.9181</v>
+        <v>57729320270.8385</v>
       </c>
       <c r="C6" t="s">
         <v>14</v>
@@ -634,10 +634,10 @@
         <v>15</v>
       </c>
       <c r="E6" t="n">
-        <v>1188540811061.7</v>
+        <v>1189679505864.58</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0484769298846796</v>
+        <v>0.0485251027577251</v>
       </c>
       <c r="G6" t="s">
         <v>16</v>
@@ -648,7 +648,7 @@
         <v>21</v>
       </c>
       <c r="B7" t="n">
-        <v>50059149532.8568</v>
+        <v>50107130956.8652</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
@@ -657,10 +657,10 @@
         <v>15</v>
       </c>
       <c r="E7" t="n">
-        <v>1188540811061.7</v>
+        <v>1189679505864.58</v>
       </c>
       <c r="F7" t="n">
-        <v>0.042118157884827</v>
+        <v>0.0421181761221066</v>
       </c>
       <c r="G7" t="s">
         <v>16</v>
@@ -671,7 +671,7 @@
         <v>13</v>
       </c>
       <c r="B8" t="n">
-        <v>1494489016.34197</v>
+        <v>1494770229.59111</v>
       </c>
       <c r="C8" t="s">
         <v>22</v>
@@ -680,10 +680,10 @@
         <v>23</v>
       </c>
       <c r="E8" t="n">
-        <v>36578258579.0119</v>
+        <v>36521769730.4009</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0408573036114815</v>
+        <v>0.0409281981849542</v>
       </c>
       <c r="G8" t="s">
         <v>24</v>
@@ -694,7 +694,7 @@
         <v>17</v>
       </c>
       <c r="B9" t="n">
-        <v>17365600409.4626</v>
+        <v>17356975844.8493</v>
       </c>
       <c r="C9" t="s">
         <v>22</v>
@@ -703,10 +703,10 @@
         <v>23</v>
       </c>
       <c r="E9" t="n">
-        <v>36578258579.0119</v>
+        <v>36521769730.4009</v>
       </c>
       <c r="F9" t="n">
-        <v>0.474751972457945</v>
+        <v>0.475250130893883</v>
       </c>
       <c r="G9" t="s">
         <v>24</v>
@@ -717,7 +717,7 @@
         <v>18</v>
       </c>
       <c r="B10" t="n">
-        <v>11258730575.8864</v>
+        <v>11245656786.8144</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
@@ -726,10 +726,10 @@
         <v>23</v>
       </c>
       <c r="E10" t="n">
-        <v>36578258579.0119</v>
+        <v>36521769730.4009</v>
       </c>
       <c r="F10" t="n">
-        <v>0.307798430359026</v>
+        <v>0.307916534982517</v>
       </c>
       <c r="G10" t="s">
         <v>24</v>
@@ -740,7 +740,7 @@
         <v>19</v>
       </c>
       <c r="B11" t="n">
-        <v>2471791612.21309</v>
+        <v>2463828549.26231</v>
       </c>
       <c r="C11" t="s">
         <v>22</v>
@@ -749,10 +749,10 @@
         <v>23</v>
       </c>
       <c r="E11" t="n">
-        <v>36578258579.0119</v>
+        <v>36521769730.4009</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0675754316426471</v>
+        <v>0.0674619156587971</v>
       </c>
       <c r="G11" t="s">
         <v>24</v>
@@ -763,7 +763,7 @@
         <v>20</v>
       </c>
       <c r="B12" t="n">
-        <v>1783927620.95191</v>
+        <v>1770512169.96196</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
@@ -772,10 +772,10 @@
         <v>23</v>
       </c>
       <c r="E12" t="n">
-        <v>36578258579.0119</v>
+        <v>36521769730.4009</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0487701626663963</v>
+        <v>0.0484782687978064</v>
       </c>
       <c r="G12" t="s">
         <v>24</v>
@@ -786,7 +786,7 @@
         <v>21</v>
       </c>
       <c r="B13" t="n">
-        <v>2203719344.15584</v>
+        <v>2190026149.92183</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
@@ -795,10 +795,10 @@
         <v>23</v>
       </c>
       <c r="E13" t="n">
-        <v>36578258579.0119</v>
+        <v>36521769730.4009</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0602466992625042</v>
+        <v>0.0599649514820428</v>
       </c>
       <c r="G13" t="s">
         <v>24</v>
@@ -1085,7 +1085,7 @@
         <v>13</v>
       </c>
       <c r="B26" t="n">
-        <v>1302819408</v>
+        <v>1302819380</v>
       </c>
       <c r="C26" t="s">
         <v>29</v>
@@ -1094,10 +1094,10 @@
         <v>23</v>
       </c>
       <c r="E26" t="n">
-        <v>7618813158</v>
+        <v>7618629943</v>
       </c>
       <c r="F26" t="n">
-        <v>0.171000309494662</v>
+        <v>0.171004418083993</v>
       </c>
       <c r="G26" t="s">
         <v>30</v>
@@ -1108,7 +1108,7 @@
         <v>17</v>
       </c>
       <c r="B27" t="n">
-        <v>3970601604</v>
+        <v>3970583353</v>
       </c>
       <c r="C27" t="s">
         <v>29</v>
@@ -1117,10 +1117,10 @@
         <v>23</v>
       </c>
       <c r="E27" t="n">
-        <v>7618813158</v>
+        <v>7618629943</v>
       </c>
       <c r="F27" t="n">
-        <v>0.521157498111204</v>
+        <v>0.521167635481255</v>
       </c>
       <c r="G27" t="s">
         <v>30</v>
@@ -1131,7 +1131,7 @@
         <v>18</v>
       </c>
       <c r="B28" t="n">
-        <v>1193017674</v>
+        <v>1192863286</v>
       </c>
       <c r="C28" t="s">
         <v>29</v>
@@ -1140,10 +1140,10 @@
         <v>23</v>
       </c>
       <c r="E28" t="n">
-        <v>7618813158</v>
+        <v>7618629943</v>
       </c>
       <c r="F28" t="n">
-        <v>0.156588388408934</v>
+        <v>0.15657188955555</v>
       </c>
       <c r="G28" t="s">
         <v>30</v>
@@ -1154,7 +1154,7 @@
         <v>19</v>
       </c>
       <c r="B29" t="n">
-        <v>249097505</v>
+        <v>249086331</v>
       </c>
       <c r="C29" t="s">
         <v>29</v>
@@ -1163,10 +1163,10 @@
         <v>23</v>
       </c>
       <c r="E29" t="n">
-        <v>7618813158</v>
+        <v>7618629943</v>
       </c>
       <c r="F29" t="n">
-        <v>0.0326950536565449</v>
+        <v>0.0326943732486785</v>
       </c>
       <c r="G29" t="s">
         <v>30</v>
@@ -1177,7 +1177,7 @@
         <v>20</v>
       </c>
       <c r="B30" t="n">
-        <v>646430843</v>
+        <v>646430786</v>
       </c>
       <c r="C30" t="s">
         <v>29</v>
@@ -1186,10 +1186,10 @@
         <v>23</v>
       </c>
       <c r="E30" t="n">
-        <v>7618813158</v>
+        <v>7618629943</v>
       </c>
       <c r="F30" t="n">
-        <v>0.084846659131052</v>
+        <v>0.0848486920662082</v>
       </c>
       <c r="G30" t="s">
         <v>30</v>
@@ -1200,7 +1200,7 @@
         <v>21</v>
       </c>
       <c r="B31" t="n">
-        <v>256846124</v>
+        <v>256846807</v>
       </c>
       <c r="C31" t="s">
         <v>29</v>
@@ -1209,10 +1209,10 @@
         <v>23</v>
       </c>
       <c r="E31" t="n">
-        <v>7618813158</v>
+        <v>7618629943</v>
       </c>
       <c r="F31" t="n">
-        <v>0.0337120911976038</v>
+        <v>0.0337129915643154</v>
       </c>
       <c r="G31" t="s">
         <v>30</v>
@@ -1223,7 +1223,7 @@
         <v>13</v>
       </c>
       <c r="B32" t="n">
-        <v>1842785560.42368</v>
+        <v>1842565311.82348</v>
       </c>
       <c r="C32" t="s">
         <v>31</v>
@@ -1232,10 +1232,10 @@
         <v>15</v>
       </c>
       <c r="E32" t="n">
-        <v>490597230718.84</v>
+        <v>490738295127.81</v>
       </c>
       <c r="F32" t="n">
-        <v>0.00375620864741443</v>
+        <v>0.00375468010162849</v>
       </c>
       <c r="G32" t="s">
         <v>32</v>
@@ -1246,7 +1246,7 @@
         <v>17</v>
       </c>
       <c r="B33" t="n">
-        <v>95046312830.2676</v>
+        <v>94976534825.3931</v>
       </c>
       <c r="C33" t="s">
         <v>31</v>
@@ -1255,10 +1255,10 @@
         <v>15</v>
       </c>
       <c r="E33" t="n">
-        <v>490597230718.84</v>
+        <v>490738295127.81</v>
       </c>
       <c r="F33" t="n">
-        <v>0.193735934242846</v>
+        <v>0.193538054332314</v>
       </c>
       <c r="G33" t="s">
         <v>32</v>
@@ -1269,7 +1269,7 @@
         <v>18</v>
       </c>
       <c r="B34" t="n">
-        <v>369870680969.589</v>
+        <v>370041679034.565</v>
       </c>
       <c r="C34" t="s">
         <v>31</v>
@@ -1278,10 +1278,10 @@
         <v>15</v>
       </c>
       <c r="E34" t="n">
-        <v>490597230718.84</v>
+        <v>490738295127.81</v>
       </c>
       <c r="F34" t="n">
-        <v>0.753919218882751</v>
+        <v>0.754050952836664</v>
       </c>
       <c r="G34" t="s">
         <v>32</v>
@@ -1292,7 +1292,7 @@
         <v>19</v>
       </c>
       <c r="B35" t="n">
-        <v>58331157.2703504</v>
+        <v>57825944.5643504</v>
       </c>
       <c r="C35" t="s">
         <v>31</v>
@@ -1301,10 +1301,10 @@
         <v>15</v>
       </c>
       <c r="E35" t="n">
-        <v>490597230718.84</v>
+        <v>490738295127.81</v>
       </c>
       <c r="F35" t="n">
-        <v>0.000118898260360911</v>
+        <v>0.000117834587474552</v>
       </c>
       <c r="G35" t="s">
         <v>32</v>
@@ -1315,7 +1315,7 @@
         <v>20</v>
       </c>
       <c r="B36" t="n">
-        <v>11923309819.3419</v>
+        <v>11944974298.2492</v>
       </c>
       <c r="C36" t="s">
         <v>31</v>
@@ -1324,10 +1324,10 @@
         <v>15</v>
       </c>
       <c r="E36" t="n">
-        <v>490597230718.84</v>
+        <v>490738295127.81</v>
       </c>
       <c r="F36" t="n">
-        <v>0.0243036631125525</v>
+        <v>0.0243408236464167</v>
       </c>
       <c r="G36" t="s">
         <v>32</v>
@@ -1338,7 +1338,7 @@
         <v>21</v>
       </c>
       <c r="B37" t="n">
-        <v>11855810381.9478</v>
+        <v>11874715713.2148</v>
       </c>
       <c r="C37" t="s">
         <v>31</v>
@@ -1347,10 +1347,10 @@
         <v>15</v>
       </c>
       <c r="E37" t="n">
-        <v>490597230718.84</v>
+        <v>490738295127.81</v>
       </c>
       <c r="F37" t="n">
-        <v>0.0241660768540748</v>
+        <v>0.0241976544955027</v>
       </c>
       <c r="G37" t="s">
         <v>32</v>
@@ -1361,7 +1361,7 @@
         <v>13</v>
       </c>
       <c r="B38" t="n">
-        <v>10255840754.2326</v>
+        <v>10293558079.3937</v>
       </c>
       <c r="C38" t="s">
         <v>33</v>
@@ -1370,10 +1370,10 @@
         <v>15</v>
       </c>
       <c r="E38" t="n">
-        <v>603901715211.91</v>
+        <v>604680080872.7</v>
       </c>
       <c r="F38" t="n">
-        <v>0.0169826322659703</v>
+        <v>0.0170231472889558</v>
       </c>
       <c r="G38" t="s">
         <v>34</v>
@@ -1384,7 +1384,7 @@
         <v>17</v>
       </c>
       <c r="B39" t="n">
-        <v>191486897486.866</v>
+        <v>192043417221.044</v>
       </c>
       <c r="C39" t="s">
         <v>33</v>
@@ -1393,10 +1393,10 @@
         <v>15</v>
       </c>
       <c r="E39" t="n">
-        <v>603901715211.91</v>
+        <v>604680080872.7</v>
       </c>
       <c r="F39" t="n">
-        <v>0.317082883958481</v>
+        <v>0.317595077621672</v>
       </c>
       <c r="G39" t="s">
         <v>34</v>
@@ -1407,7 +1407,7 @@
         <v>18</v>
       </c>
       <c r="B40" t="n">
-        <v>227049863979.87</v>
+        <v>227105692972.81</v>
       </c>
       <c r="C40" t="s">
         <v>33</v>
@@ -1416,10 +1416,10 @@
         <v>15</v>
       </c>
       <c r="E40" t="n">
-        <v>603901715211.91</v>
+        <v>604680080872.7</v>
       </c>
       <c r="F40" t="n">
-        <v>0.37597155010596</v>
+        <v>0.375579914332619</v>
       </c>
       <c r="G40" t="s">
         <v>34</v>
@@ -1430,7 +1430,7 @@
         <v>19</v>
       </c>
       <c r="B41" t="n">
-        <v>102878984127.703</v>
+        <v>102898575536.138</v>
       </c>
       <c r="C41" t="s">
         <v>33</v>
@@ -1439,10 +1439,10 @@
         <v>15</v>
       </c>
       <c r="E41" t="n">
-        <v>603901715211.91</v>
+        <v>604680080872.7</v>
       </c>
       <c r="F41" t="n">
-        <v>0.170357164976097</v>
+        <v>0.170170274813138</v>
       </c>
       <c r="G41" t="s">
         <v>34</v>
@@ -1453,7 +1453,7 @@
         <v>20</v>
       </c>
       <c r="B42" t="n">
-        <v>40141595871.0142</v>
+        <v>40225847241.0209</v>
       </c>
       <c r="C42" t="s">
         <v>33</v>
@@ -1462,10 +1462,10 @@
         <v>15</v>
       </c>
       <c r="E42" t="n">
-        <v>603901715211.91</v>
+        <v>604680080872.7</v>
       </c>
       <c r="F42" t="n">
-        <v>0.0664704120883783</v>
+        <v>0.0665241811553726</v>
       </c>
       <c r="G42" t="s">
         <v>34</v>
@@ -1476,7 +1476,7 @@
         <v>21</v>
       </c>
       <c r="B43" t="n">
-        <v>32088532992.2242</v>
+        <v>32112989822.2935</v>
       </c>
       <c r="C43" t="s">
         <v>33</v>
@@ -1485,10 +1485,10 @@
         <v>15</v>
       </c>
       <c r="E43" t="n">
-        <v>603901715211.91</v>
+        <v>604680080872.7</v>
       </c>
       <c r="F43" t="n">
-        <v>0.0531353566051129</v>
+        <v>0.0531074047882421</v>
       </c>
       <c r="G43" t="s">
         <v>34</v>
@@ -1499,7 +1499,7 @@
         <v>13</v>
       </c>
       <c r="B44" t="n">
-        <v>29078077230.3964</v>
+        <v>29105323452.7362</v>
       </c>
       <c r="C44" t="s">
         <v>35</v>
@@ -1508,10 +1508,10 @@
         <v>15</v>
       </c>
       <c r="E44" t="n">
-        <v>94041865130.9464</v>
+        <v>94261129864.0724</v>
       </c>
       <c r="F44" t="n">
-        <v>0.309203535998646</v>
+        <v>0.308773335251837</v>
       </c>
       <c r="G44" t="s">
         <v>36</v>
@@ -1522,7 +1522,7 @@
         <v>17</v>
       </c>
       <c r="B45" t="n">
-        <v>39516892081.3188</v>
+        <v>39692849357.9866</v>
       </c>
       <c r="C45" t="s">
         <v>35</v>
@@ -1531,10 +1531,10 @@
         <v>15</v>
       </c>
       <c r="E45" t="n">
-        <v>94041865130.9464</v>
+        <v>94261129864.0724</v>
       </c>
       <c r="F45" t="n">
-        <v>0.420205320537766</v>
+        <v>0.421094563742499</v>
       </c>
       <c r="G45" t="s">
         <v>36</v>
@@ -1545,7 +1545,7 @@
         <v>18</v>
       </c>
       <c r="B46" t="n">
-        <v>2051310892.99176</v>
+        <v>2054366192.54176</v>
       </c>
       <c r="C46" t="s">
         <v>35</v>
@@ -1554,10 +1554,10 @@
         <v>15</v>
       </c>
       <c r="E46" t="n">
-        <v>94041865130.9464</v>
+        <v>94261129864.0724</v>
       </c>
       <c r="F46" t="n">
-        <v>0.0218127414863099</v>
+        <v>0.0217944151051894</v>
       </c>
       <c r="G46" t="s">
         <v>36</v>
@@ -1568,7 +1568,7 @@
         <v>19</v>
       </c>
       <c r="B47" t="n">
-        <v>11728874894.9925</v>
+        <v>11730666707.8825</v>
       </c>
       <c r="C47" t="s">
         <v>35</v>
@@ -1577,10 +1577,10 @@
         <v>15</v>
       </c>
       <c r="E47" t="n">
-        <v>94041865130.9464</v>
+        <v>94261129864.0724</v>
       </c>
       <c r="F47" t="n">
-        <v>0.124719717953923</v>
+        <v>0.124448611265307</v>
       </c>
       <c r="G47" t="s">
         <v>36</v>
@@ -1591,7 +1591,7 @@
         <v>20</v>
       </c>
       <c r="B48" t="n">
-        <v>5551903872.56207</v>
+        <v>5558498731.56837</v>
       </c>
       <c r="C48" t="s">
         <v>35</v>
@@ -1600,10 +1600,10 @@
         <v>15</v>
       </c>
       <c r="E48" t="n">
-        <v>94041865130.9464</v>
+        <v>94261129864.0724</v>
       </c>
       <c r="F48" t="n">
-        <v>0.0590365138423344</v>
+        <v>0.0589691502699353</v>
       </c>
       <c r="G48" t="s">
         <v>36</v>
@@ -1614,7 +1614,7 @@
         <v>21</v>
       </c>
       <c r="B49" t="n">
-        <v>6114806158.68487</v>
+        <v>6119425421.35697</v>
       </c>
       <c r="C49" t="s">
         <v>35</v>
@@ -1623,10 +1623,10 @@
         <v>15</v>
       </c>
       <c r="E49" t="n">
-        <v>94041865130.9464</v>
+        <v>94261129864.0724</v>
       </c>
       <c r="F49" t="n">
-        <v>0.0650221701810194</v>
+        <v>0.0649199243652329</v>
       </c>
       <c r="G49" t="s">
         <v>36</v>
@@ -1637,7 +1637,7 @@
         <v>13</v>
       </c>
       <c r="B50" t="n">
-        <v>3227053166.38986</v>
+        <v>3433150433.67798</v>
       </c>
       <c r="C50" t="s">
         <v>37</v>
@@ -1646,10 +1646,10 @@
         <v>23</v>
       </c>
       <c r="E50" t="n">
-        <v>50317225379.5558</v>
+        <v>51126029486.308</v>
       </c>
       <c r="F50" t="n">
-        <v>0.0641341636397351</v>
+        <v>0.0671507345313685</v>
       </c>
       <c r="G50" t="s">
         <v>38</v>
@@ -1660,7 +1660,7 @@
         <v>17</v>
       </c>
       <c r="B51" t="n">
-        <v>22708417480.4679</v>
+        <v>23078805804.8676</v>
       </c>
       <c r="C51" t="s">
         <v>37</v>
@@ -1669,10 +1669,10 @@
         <v>23</v>
       </c>
       <c r="E51" t="n">
-        <v>50317225379.5558</v>
+        <v>51126029486.308</v>
       </c>
       <c r="F51" t="n">
-        <v>0.451305041348614</v>
+        <v>0.45141009455953</v>
       </c>
       <c r="G51" t="s">
         <v>38</v>
@@ -1683,7 +1683,7 @@
         <v>18</v>
       </c>
       <c r="B52" t="n">
-        <v>14241088068.0732</v>
+        <v>14284243064.0032</v>
       </c>
       <c r="C52" t="s">
         <v>37</v>
@@ -1692,10 +1692,10 @@
         <v>23</v>
       </c>
       <c r="E52" t="n">
-        <v>50317225379.5558</v>
+        <v>51126029486.308</v>
       </c>
       <c r="F52" t="n">
-        <v>0.283026100120764</v>
+        <v>0.279392771305049</v>
       </c>
       <c r="G52" t="s">
         <v>38</v>
@@ -1706,7 +1706,7 @@
         <v>19</v>
       </c>
       <c r="B53" t="n">
-        <v>3417590169.24149</v>
+        <v>3416156396.33553</v>
       </c>
       <c r="C53" t="s">
         <v>37</v>
@@ -1715,10 +1715,10 @@
         <v>23</v>
       </c>
       <c r="E53" t="n">
-        <v>50317225379.5558</v>
+        <v>51126029486.308</v>
       </c>
       <c r="F53" t="n">
-        <v>0.0679208788533495</v>
+        <v>0.0668183395162813</v>
       </c>
       <c r="G53" t="s">
         <v>38</v>
@@ -1729,7 +1729,7 @@
         <v>20</v>
       </c>
       <c r="B54" t="n">
-        <v>3611566163.60705</v>
+        <v>3695402314.40367</v>
       </c>
       <c r="C54" t="s">
         <v>37</v>
@@ -1738,10 +1738,10 @@
         <v>23</v>
       </c>
       <c r="E54" t="n">
-        <v>50317225379.5558</v>
+        <v>51126029486.308</v>
       </c>
       <c r="F54" t="n">
-        <v>0.0717759402742119</v>
+        <v>0.072280252378944</v>
       </c>
       <c r="G54" t="s">
         <v>38</v>
@@ -1752,7 +1752,7 @@
         <v>21</v>
       </c>
       <c r="B55" t="n">
-        <v>3111510331.77624</v>
+        <v>3218271473.01995</v>
       </c>
       <c r="C55" t="s">
         <v>37</v>
@@ -1761,10 +1761,10 @@
         <v>23</v>
       </c>
       <c r="E55" t="n">
-        <v>50317225379.5558</v>
+        <v>51126029486.308</v>
       </c>
       <c r="F55" t="n">
-        <v>0.061837875763326</v>
+        <v>0.0629478077088273</v>
       </c>
       <c r="G55" t="s">
         <v>38</v>
@@ -1775,7 +1775,7 @@
         <v>13</v>
       </c>
       <c r="B56" t="n">
-        <v>5002955654.38453</v>
+        <v>5209052921.67265</v>
       </c>
       <c r="C56" t="s">
         <v>39</v>
@@ -1784,10 +1784,10 @@
         <v>23</v>
       </c>
       <c r="E56" t="n">
-        <v>56922264227.1558</v>
+        <v>57731068333.908</v>
       </c>
       <c r="F56" t="n">
-        <v>0.0878910163239392</v>
+        <v>0.0902296297644149</v>
       </c>
       <c r="G56" t="s">
         <v>40</v>
@@ -1798,7 +1798,7 @@
         <v>17</v>
       </c>
       <c r="B57" t="n">
-        <v>25347914312.6279</v>
+        <v>25718302637.0276</v>
       </c>
       <c r="C57" t="s">
         <v>39</v>
@@ -1807,10 +1807,10 @@
         <v>23</v>
       </c>
       <c r="E57" t="n">
-        <v>56922264227.1558</v>
+        <v>57731068333.908</v>
       </c>
       <c r="F57" t="n">
-        <v>0.445307555080271</v>
+        <v>0.445484613038455</v>
       </c>
       <c r="G57" t="s">
         <v>40</v>
@@ -1821,7 +1821,7 @@
         <v>18</v>
       </c>
       <c r="B58" t="n">
-        <v>14099863291.7532</v>
+        <v>14143018287.6832</v>
       </c>
       <c r="C58" t="s">
         <v>39</v>
@@ -1830,10 +1830,10 @@
         <v>23</v>
       </c>
       <c r="E58" t="n">
-        <v>56922264227.1558</v>
+        <v>57731068333.908</v>
       </c>
       <c r="F58" t="n">
-        <v>0.247703837561447</v>
+        <v>0.244981059520363</v>
       </c>
       <c r="G58" t="s">
         <v>40</v>
@@ -1844,7 +1844,7 @@
         <v>19</v>
       </c>
       <c r="B59" t="n">
-        <v>3506879515.27349</v>
+        <v>3505445742.36753</v>
       </c>
       <c r="C59" t="s">
         <v>39</v>
@@ -1853,10 +1853,10 @@
         <v>23</v>
       </c>
       <c r="E59" t="n">
-        <v>56922264227.1558</v>
+        <v>57731068333.908</v>
       </c>
       <c r="F59" t="n">
-        <v>0.0616082224220531</v>
+        <v>0.0607202645565565</v>
       </c>
       <c r="G59" t="s">
         <v>40</v>
@@ -1867,7 +1867,7 @@
         <v>20</v>
       </c>
       <c r="B60" t="n">
-        <v>5854671636.42838</v>
+        <v>5938507787.225</v>
       </c>
       <c r="C60" t="s">
         <v>39</v>
@@ -1876,10 +1876,10 @@
         <v>23</v>
       </c>
       <c r="E60" t="n">
-        <v>56922264227.1558</v>
+        <v>57731068333.908</v>
       </c>
       <c r="F60" t="n">
-        <v>0.102853808012003</v>
+        <v>0.102865024996204</v>
       </c>
       <c r="G60" t="s">
         <v>40</v>
@@ -1890,7 +1890,7 @@
         <v>21</v>
       </c>
       <c r="B61" t="n">
-        <v>3109979816.68824</v>
+        <v>3216740957.93195</v>
       </c>
       <c r="C61" t="s">
         <v>39</v>
@@ -1899,10 +1899,10 @@
         <v>23</v>
       </c>
       <c r="E61" t="n">
-        <v>56922264227.1558</v>
+        <v>57731068333.908</v>
       </c>
       <c r="F61" t="n">
-        <v>0.0546355606002857</v>
+        <v>0.0557194081240069</v>
       </c>
       <c r="G61" t="s">
         <v>40</v>

</xml_diff>

<commit_message>
budget analysis and equity figure
</commit_message>
<xml_diff>
--- a/Results/Plot data/ipcc_ar6_figure_equity_perspectives.xlsx
+++ b/Results/Plot data/ipcc_ar6_figure_equity_perspectives.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t xml:space="preserve">Author</t>
   </si>
@@ -24,7 +24,7 @@
     <t xml:space="preserve">Last update</t>
   </si>
   <si>
-    <t xml:space="preserve">2021-10-19 11:26:23</t>
+    <t xml:space="preserve">2021-10-20 15:11:36</t>
   </si>
   <si>
     <t xml:space="preserve">Code</t>
@@ -33,7 +33,7 @@
     <t xml:space="preserve">https://github.com/mcc-apsis/AR6-Emissions-trends-and-drivers/blob/master/R/Analysis%20and%20figures/equity_perspectives.Rmd</t>
   </si>
   <si>
-    <t xml:space="preserve">region_select</t>
+    <t xml:space="preserve">region_ar6_6</t>
   </si>
   <si>
     <t xml:space="preserve">value</t>
@@ -120,13 +120,19 @@
     <t xml:space="preserve">Territorial CO2, excl. LULUCF (1750-2019)</t>
   </si>
   <si>
-    <t xml:space="preserve">1614 Gt CO2eq</t>
+    <t xml:space="preserve">1612 Gt CO2eq</t>
   </si>
   <si>
     <t xml:space="preserve">Territorial CO2, incl. LULUCF (1850-2019)</t>
   </si>
   <si>
-    <t xml:space="preserve">2372 Gt CO2eq</t>
+    <t xml:space="preserve">2370 Gt CO2eq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Territorial CO2, excl. LULUCF (1850-2019)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1607 Gt CO2eq</t>
   </si>
   <si>
     <t xml:space="preserve">Latin America and Caribbean</t>
@@ -661,7 +667,7 @@
         <v>15</v>
       </c>
       <c r="B6" t="n">
-        <v>1881528439.69866</v>
+        <v>1882897819.93133</v>
       </c>
       <c r="C6" t="s">
         <v>26</v>
@@ -670,19 +676,19 @@
         <v>20</v>
       </c>
       <c r="E6" t="n">
-        <v>33711877353.0725</v>
+        <v>34010118873.7897</v>
       </c>
       <c r="F6" t="n">
-        <v>0.0558120338417514</v>
+        <v>0.0553628708831833</v>
       </c>
       <c r="G6" t="s">
         <v>27</v>
       </c>
       <c r="H6" t="n">
-        <v>0.0558120338417514</v>
+        <v>0.0553628708831833</v>
       </c>
       <c r="I6" t="n">
-        <v>0.0279060169208757</v>
+        <v>0.0276814354415917</v>
       </c>
     </row>
     <row r="7">
@@ -777,7 +783,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="n">
-        <v>55.4526506499863</v>
+        <v>55.9783077</v>
       </c>
       <c r="C10" t="s">
         <v>34</v>
@@ -786,19 +792,19 @@
         <v>17</v>
       </c>
       <c r="E10" t="n">
-        <v>1613.7765720005</v>
+        <v>1611.753827743</v>
       </c>
       <c r="F10" t="n">
-        <v>0.0343620372312415</v>
+        <v>0.0347313012300325</v>
       </c>
       <c r="G10" t="s">
         <v>35</v>
       </c>
       <c r="H10" t="n">
-        <v>0.0343620372312415</v>
+        <v>0.0347313012300325</v>
       </c>
       <c r="I10" t="n">
-        <v>0.0171810186156207</v>
+        <v>0.0173656506150162</v>
       </c>
     </row>
     <row r="11">
@@ -806,7 +812,7 @@
         <v>15</v>
       </c>
       <c r="B11" t="n">
-        <v>56.9274139524717</v>
+        <v>57.4530710024853</v>
       </c>
       <c r="C11" t="s">
         <v>36</v>
@@ -815,1469 +821,1643 @@
         <v>17</v>
       </c>
       <c r="E11" t="n">
-        <v>2371.79921725908</v>
+        <v>2369.77043627992</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0240017846106967</v>
+        <v>0.0242441504556346</v>
       </c>
       <c r="G11" t="s">
         <v>37</v>
       </c>
       <c r="H11" t="n">
-        <v>0.0240017846106967</v>
+        <v>0.0242441504556346</v>
       </c>
       <c r="I11" t="n">
-        <v>0.0120008923053484</v>
+        <v>0.0121220752278173</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12" t="n">
+        <v>55.9783077</v>
+      </c>
+      <c r="C12" t="s">
         <v>38</v>
       </c>
-      <c r="B12" t="n">
-        <v>60004567655.2182</v>
-      </c>
-      <c r="C12" t="s">
-        <v>16</v>
-      </c>
       <c r="D12" t="s">
         <v>17</v>
       </c>
       <c r="E12" t="n">
-        <v>1238053003179.45</v>
+        <v>1607.191308688</v>
       </c>
       <c r="F12" t="n">
-        <v>0.0484668810633473</v>
+        <v>0.034829896974553</v>
       </c>
       <c r="G12" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="H12" t="n">
-        <v>0.0907083335475968</v>
+        <v>0.034829896974553</v>
       </c>
       <c r="I12" t="n">
-        <v>0.0664748930159231</v>
+        <v>0.0174149484872765</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B13" t="n">
-        <v>1770512169.96196</v>
+        <v>60004567655.2182</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E13" t="n">
-        <v>36521769730.4009</v>
+        <v>1238053003179.45</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0484782687978064</v>
+        <v>0.0484668810633473</v>
       </c>
       <c r="G13" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="H13" t="n">
-        <v>0.108443220279849</v>
+        <v>0.0907083335475968</v>
       </c>
       <c r="I13" t="n">
-        <v>0.084204085880946</v>
+        <v>0.0664748930159231</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B14" t="n">
-        <v>202792190134.539</v>
+        <v>1770512169.96196</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E14" t="n">
-        <v>762579127591.92</v>
+        <v>36521769730.4009</v>
       </c>
       <c r="F14" t="n">
-        <v>0.26592937414235</v>
+        <v>0.0484782687978064</v>
       </c>
       <c r="G14" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H14" t="n">
-        <v>0.267863289258992</v>
+        <v>0.108443220279849</v>
       </c>
       <c r="I14" t="n">
-        <v>0.134898602187817</v>
+        <v>0.084204085880946</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B15" t="n">
-        <v>2243105472.82133</v>
+        <v>202792190134.539</v>
       </c>
       <c r="C15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E15" t="n">
-        <v>6605038847.6</v>
+        <v>762579127591.92</v>
       </c>
       <c r="F15" t="n">
-        <v>0.339605190003748</v>
+        <v>0.26592937414235</v>
       </c>
       <c r="G15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="H15" t="n">
-        <v>0.33937347068713</v>
+        <v>0.267863289258992</v>
       </c>
       <c r="I15" t="n">
-        <v>0.169570875685256</v>
+        <v>0.134898602187817</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B16" t="n">
-        <v>1804646774.18749</v>
+        <v>2243105472.82133</v>
       </c>
       <c r="C16" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
       </c>
       <c r="E16" t="n">
-        <v>33711877353.0725</v>
+        <v>6605038847.6</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0535314825480347</v>
+        <v>0.339605190003748</v>
       </c>
       <c r="G16" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H16" t="n">
-        <v>0.109343516389786</v>
+        <v>0.33937347068713</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0825777751157688</v>
+        <v>0.169570875685256</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B17" t="n">
-        <v>646430786</v>
+        <v>1805960199.78733</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D17" t="s">
         <v>20</v>
       </c>
       <c r="E17" t="n">
-        <v>7618629943</v>
+        <v>34010118873.7897</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0848486920662082</v>
+        <v>0.0531006729641019</v>
       </c>
       <c r="G17" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H17" t="n">
-        <v>0.118561683630524</v>
+        <v>0.108463543847285</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0761373375974195</v>
+        <v>0.0819132073652342</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B18" t="n">
-        <v>3672431568.80367</v>
+        <v>646430786</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D18" t="s">
         <v>20</v>
       </c>
       <c r="E18" t="n">
-        <v>51044144755.8797</v>
+        <v>7618629943</v>
       </c>
       <c r="F18" t="n">
-        <v>0.071946186705002</v>
+        <v>0.0848486920662082</v>
       </c>
       <c r="G18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H18" t="n">
-        <v>0.134960954216597</v>
+        <v>0.118561683630524</v>
       </c>
       <c r="I18" t="n">
-        <v>0.0989878608640957</v>
+        <v>0.0761373375974195</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B19" t="n">
-        <v>5915537041.625</v>
+        <v>3672431568.80367</v>
       </c>
       <c r="C19" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
         <v>20</v>
       </c>
       <c r="E19" t="n">
-        <v>57649183603.4797</v>
+        <v>51044144755.8797</v>
       </c>
       <c r="F19" t="n">
-        <v>0.102612676743404</v>
+        <v>0.071946186705002</v>
       </c>
       <c r="G19" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H19" t="n">
-        <v>0.158381105688474</v>
+        <v>0.134960954216597</v>
       </c>
       <c r="I19" t="n">
-        <v>0.107074767316772</v>
+        <v>0.0989878608640957</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B20" t="n">
-        <v>69.7469431238433</v>
+        <v>5915537041.625</v>
       </c>
       <c r="C20" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D20" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E20" t="n">
-        <v>1613.7765720005</v>
+        <v>57649183603.4797</v>
       </c>
       <c r="F20" t="n">
-        <v>0.0432197023639911</v>
+        <v>0.102612676743404</v>
       </c>
       <c r="G20" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H20" t="n">
-        <v>0.0775817395952326</v>
+        <v>0.158381105688474</v>
       </c>
       <c r="I20" t="n">
-        <v>0.055971888413237</v>
+        <v>0.107074767316772</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B21" t="n">
-        <v>272.539133258382</v>
+        <v>68.456694403</v>
       </c>
       <c r="C21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
         <v>17</v>
       </c>
       <c r="E21" t="n">
-        <v>2371.79921725908</v>
+        <v>1611.753827743</v>
       </c>
       <c r="F21" t="n">
-        <v>0.114908180791684</v>
+        <v>0.0424734182259474</v>
       </c>
       <c r="G21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H21" t="n">
-        <v>0.138909965402381</v>
+        <v>0.0772047194559799</v>
       </c>
       <c r="I21" t="n">
-        <v>0.0814558750065388</v>
+        <v>0.0559680103430062</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B22" t="n">
-        <v>120067434799.314</v>
+        <v>271.248884537539</v>
       </c>
       <c r="C22" t="s">
-        <v>16</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
       </c>
       <c r="E22" t="n">
-        <v>1238053003179.45</v>
+        <v>2369.77043627992</v>
       </c>
       <c r="F22" t="n">
-        <v>0.0969808517817638</v>
+        <v>0.114462093198929</v>
       </c>
       <c r="G22" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="H22" t="n">
-        <v>0.187689185329361</v>
+        <v>0.138706243654564</v>
       </c>
       <c r="I22" t="n">
-        <v>0.139198759438479</v>
+        <v>0.0814751970550992</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
+        <v>40</v>
+      </c>
+      <c r="B23" t="n">
+        <v>68.456694403</v>
+      </c>
+      <c r="C23" t="s">
+        <v>38</v>
+      </c>
+      <c r="D23" t="s">
+        <v>17</v>
+      </c>
+      <c r="E23" t="n">
+        <v>1607.191308688</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0.0425939924095802</v>
+      </c>
+      <c r="G23" t="s">
         <v>39</v>
       </c>
-      <c r="B23" t="n">
-        <v>2463828549.26231</v>
-      </c>
-      <c r="C23" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" t="s">
-        <v>20</v>
-      </c>
-      <c r="E23" t="n">
-        <v>36521769730.4009</v>
-      </c>
-      <c r="F23" t="n">
-        <v>0.0674619156587971</v>
-      </c>
-      <c r="G23" t="s">
-        <v>21</v>
-      </c>
       <c r="H23" t="n">
-        <v>0.175905135938646</v>
+        <v>0.0774238893841332</v>
       </c>
       <c r="I23" t="n">
-        <v>0.142174178109248</v>
+        <v>0.0561268931793431</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B24" t="n">
-        <v>66720368724.5653</v>
+        <v>120067434799.314</v>
       </c>
       <c r="C24" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
       </c>
       <c r="E24" t="n">
-        <v>762579127591.92</v>
+        <v>1238053003179.45</v>
       </c>
       <c r="F24" t="n">
-        <v>0.0874930434239075</v>
+        <v>0.0969808517817638</v>
       </c>
       <c r="G24" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="H24" t="n">
-        <v>0.355356332682899</v>
+        <v>0.187689185329361</v>
       </c>
       <c r="I24" t="n">
-        <v>0.311609810970945</v>
+        <v>0.139198759438479</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B25" t="n">
-        <v>89289346.032</v>
+        <v>2463828549.26231</v>
       </c>
       <c r="C25" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="D25" t="s">
         <v>20</v>
       </c>
       <c r="E25" t="n">
-        <v>6605038847.6</v>
+        <v>36521769730.4009</v>
       </c>
       <c r="F25" t="n">
-        <v>0.0135183680357072</v>
+        <v>0.0674619156587971</v>
       </c>
       <c r="G25" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="H25" t="n">
-        <v>0.352891838722837</v>
+        <v>0.175905135938646</v>
       </c>
       <c r="I25" t="n">
-        <v>0.346132654704984</v>
+        <v>0.142174178109248</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B26" t="n">
-        <v>1790108676.09424</v>
+        <v>66720368724.5653</v>
       </c>
       <c r="C26" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E26" t="n">
-        <v>33711877353.0725</v>
+        <v>762579127591.92</v>
       </c>
       <c r="F26" t="n">
-        <v>0.0531002369682948</v>
+        <v>0.0874930434239075</v>
       </c>
       <c r="G26" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="H26" t="n">
-        <v>0.162443753358081</v>
+        <v>0.355356332682899</v>
       </c>
       <c r="I26" t="n">
-        <v>0.135893634873934</v>
+        <v>0.311609810970945</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B27" t="n">
-        <v>249086331</v>
+        <v>89289346.032</v>
       </c>
       <c r="C27" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
         <v>20</v>
       </c>
       <c r="E27" t="n">
-        <v>7618629943</v>
+        <v>6605038847.6</v>
       </c>
       <c r="F27" t="n">
-        <v>0.0326943732486785</v>
+        <v>0.0135183680357072</v>
       </c>
       <c r="G27" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="H27" t="n">
-        <v>0.151256056879202</v>
+        <v>0.352891838722837</v>
       </c>
       <c r="I27" t="n">
-        <v>0.134908870254863</v>
+        <v>0.346132654704984</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B28" t="n">
-        <v>3406964482.73553</v>
+        <v>1791411520.83667</v>
       </c>
       <c r="C28" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="D28" t="s">
         <v>20</v>
       </c>
       <c r="E28" t="n">
-        <v>51044144755.8797</v>
+        <v>34010118873.7897</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0667454513936799</v>
+        <v>0.0526728979538275</v>
       </c>
       <c r="G28" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="H28" t="n">
-        <v>0.201706405610277</v>
+        <v>0.161136441801113</v>
       </c>
       <c r="I28" t="n">
-        <v>0.168333679913437</v>
+        <v>0.134799992824199</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B29" t="n">
-        <v>3496253828.76753</v>
+        <v>249086331</v>
       </c>
       <c r="C29" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D29" t="s">
         <v>20</v>
       </c>
       <c r="E29" t="n">
-        <v>57649183603.4797</v>
+        <v>7618629943</v>
       </c>
       <c r="F29" t="n">
-        <v>0.0606470657557846</v>
+        <v>0.0326943732486785</v>
       </c>
       <c r="G29" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="H29" t="n">
-        <v>0.219028171444258</v>
+        <v>0.151256056879202</v>
       </c>
       <c r="I29" t="n">
-        <v>0.188704638566366</v>
+        <v>0.134908870254863</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B30" t="n">
-        <v>149.231345686853</v>
+        <v>3406964482.73553</v>
       </c>
       <c r="C30" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D30" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E30" t="n">
-        <v>1613.7765720005</v>
+        <v>51044144755.8797</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0924733623452351</v>
+        <v>0.0667454513936799</v>
       </c>
       <c r="G30" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="H30" t="n">
-        <v>0.170055101940468</v>
+        <v>0.201706405610277</v>
       </c>
       <c r="I30" t="n">
-        <v>0.12381842076785</v>
+        <v>0.168333679913437</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B31" t="n">
-        <v>215.951656273784</v>
+        <v>3496253828.76753</v>
       </c>
       <c r="C31" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D31" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E31" t="n">
-        <v>2371.79921725908</v>
+        <v>57649183603.4797</v>
       </c>
       <c r="F31" t="n">
-        <v>0.0910497206940407</v>
+        <v>0.0606470657557846</v>
       </c>
       <c r="G31" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="H31" t="n">
-        <v>0.229959686096422</v>
+        <v>0.219028171444258</v>
       </c>
       <c r="I31" t="n">
-        <v>0.184434825749401</v>
+        <v>0.188704638566366</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B32" t="n">
-        <v>610480923704.844</v>
+        <v>148.968879981</v>
       </c>
       <c r="C32" t="s">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D32" t="s">
         <v>17</v>
       </c>
       <c r="E32" t="n">
-        <v>1238053003179.45</v>
+        <v>1611.753827743</v>
       </c>
       <c r="F32" t="n">
-        <v>0.493097567016167</v>
+        <v>0.0924265712398566</v>
       </c>
       <c r="G32" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="H32" t="n">
-        <v>0.680786752345527</v>
+        <v>0.169631290695836</v>
       </c>
       <c r="I32" t="n">
-        <v>0.434237968837444</v>
+        <v>0.123418005075908</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B33" t="n">
-        <v>11245656786.8144</v>
+        <v>215.689190598565</v>
       </c>
       <c r="C33" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D33" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E33" t="n">
-        <v>36521769730.4009</v>
+        <v>2369.77043627992</v>
       </c>
       <c r="F33" t="n">
-        <v>0.307916534982517</v>
+        <v>0.0910169134091973</v>
       </c>
       <c r="G33" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="H33" t="n">
-        <v>0.483821670921163</v>
+        <v>0.229723157063761</v>
       </c>
       <c r="I33" t="n">
-        <v>0.329863403429905</v>
+        <v>0.184214700359162</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B34" t="n">
-        <v>152318292712.496</v>
+        <v>148.968821874</v>
       </c>
       <c r="C34" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D34" t="s">
         <v>17</v>
       </c>
       <c r="E34" t="n">
-        <v>762579127591.92</v>
+        <v>1607.191308688</v>
       </c>
       <c r="F34" t="n">
-        <v>0.199740967463256</v>
+        <v>0.0926889170372679</v>
       </c>
       <c r="G34" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="H34" t="n">
-        <v>0.555097300146155</v>
+        <v>0.170112806421401</v>
       </c>
       <c r="I34" t="n">
-        <v>0.455226816414527</v>
+        <v>0.123768347902767</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B35" t="n">
-        <v>-141224776.32</v>
+        <v>610480923704.844</v>
       </c>
       <c r="C35" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="D35" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E35" t="n">
-        <v>6605038847.6</v>
+        <v>1238053003179.45</v>
       </c>
       <c r="F35" t="n">
-        <v>-0.0213813695238621</v>
+        <v>0.493097567016167</v>
       </c>
       <c r="G35" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="H35" t="n">
-        <v>0.331510469198975</v>
+        <v>0.680786752345527</v>
       </c>
       <c r="I35" t="n">
-        <v>0.342201153960906</v>
+        <v>0.434237968837444</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B36" t="n">
-        <v>12944620056.7632</v>
+        <v>11245656786.8144</v>
       </c>
       <c r="C36" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="D36" t="s">
         <v>20</v>
       </c>
       <c r="E36" t="n">
-        <v>33711877353.0725</v>
+        <v>36521769730.4009</v>
       </c>
       <c r="F36" t="n">
-        <v>0.383978024160184</v>
+        <v>0.307916534982517</v>
       </c>
       <c r="G36" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="H36" t="n">
-        <v>0.546421777518265</v>
+        <v>0.483821670921163</v>
       </c>
       <c r="I36" t="n">
-        <v>0.354432765438173</v>
+        <v>0.329863403429905</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B37" t="n">
-        <v>1192863286</v>
+        <v>152318292712.496</v>
       </c>
       <c r="C37" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D37" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E37" t="n">
-        <v>7618629943</v>
+        <v>762579127591.92</v>
       </c>
       <c r="F37" t="n">
-        <v>0.15657188955555</v>
+        <v>0.199740967463256</v>
       </c>
       <c r="G37" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="H37" t="n">
-        <v>0.307827946434752</v>
+        <v>0.555097300146155</v>
       </c>
       <c r="I37" t="n">
-        <v>0.229542001656977</v>
+        <v>0.455226816414527</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B38" t="n">
-        <v>14251665877.1032</v>
+        <v>-141224776.32</v>
       </c>
       <c r="C38" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D38" t="s">
         <v>20</v>
       </c>
       <c r="E38" t="n">
-        <v>51044144755.8797</v>
+        <v>6605038847.6</v>
       </c>
       <c r="F38" t="n">
-        <v>0.279202755678683</v>
+        <v>-0.0213813695238621</v>
       </c>
       <c r="G38" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="H38" t="n">
-        <v>0.48090916128896</v>
+        <v>0.331510469198975</v>
       </c>
       <c r="I38" t="n">
-        <v>0.341307783449618</v>
+        <v>0.342201153960906</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B39" t="n">
-        <v>14110441100.7832</v>
+        <v>12954041177.6197</v>
       </c>
       <c r="C39" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="D39" t="s">
         <v>20</v>
       </c>
       <c r="E39" t="n">
-        <v>57649183603.4797</v>
+        <v>34010118873.7897</v>
       </c>
       <c r="F39" t="n">
-        <v>0.244763936256879</v>
+        <v>0.380887853573569</v>
       </c>
       <c r="G39" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="H39" t="n">
-        <v>0.463792107701137</v>
+        <v>0.542024295374681</v>
       </c>
       <c r="I39" t="n">
-        <v>0.341410139572698</v>
+        <v>0.351580368587897</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B40" t="n">
-        <v>943.324322096976</v>
+        <v>1192863286</v>
       </c>
       <c r="C40" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D40" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E40" t="n">
-        <v>1613.7765720005</v>
+        <v>7618629943</v>
       </c>
       <c r="F40" t="n">
-        <v>0.584544563642782</v>
+        <v>0.15657188955555</v>
       </c>
       <c r="G40" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="H40" t="n">
-        <v>0.75459966558325</v>
+        <v>0.307827946434752</v>
       </c>
       <c r="I40" t="n">
-        <v>0.462327383761859</v>
+        <v>0.229542001656977</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B41" t="n">
-        <v>1091.08619061377</v>
+        <v>14251665877.1032</v>
       </c>
       <c r="C41" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D41" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E41" t="n">
-        <v>2371.79921725908</v>
+        <v>51044144755.8797</v>
       </c>
       <c r="F41" t="n">
-        <v>0.460024686185141</v>
+        <v>0.279202755678683</v>
       </c>
       <c r="G41" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="H41" t="n">
-        <v>0.689984372281563</v>
+        <v>0.48090916128896</v>
       </c>
       <c r="I41" t="n">
-        <v>0.459972029188992</v>
+        <v>0.341307783449618</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B42" t="n">
-        <v>352380229527.506</v>
+        <v>14110441100.7832</v>
       </c>
       <c r="C42" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="D42" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E42" t="n">
-        <v>1238053003179.45</v>
+        <v>57649183603.4797</v>
       </c>
       <c r="F42" t="n">
-        <v>0.28462451011593</v>
+        <v>0.244763936256879</v>
       </c>
       <c r="G42" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="H42" t="n">
-        <v>0.965411262461457</v>
+        <v>0.463792107701137</v>
       </c>
       <c r="I42" t="n">
-        <v>0.823099007403492</v>
+        <v>0.341410139572698</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B43" t="n">
-        <v>17356975844.8493</v>
+        <v>942.860701435</v>
       </c>
       <c r="C43" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="D43" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E43" t="n">
-        <v>36521769730.4009</v>
+        <v>1611.753827743</v>
       </c>
       <c r="F43" t="n">
-        <v>0.475250130893883</v>
+        <v>0.584990514807912</v>
       </c>
       <c r="G43" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="H43" t="n">
-        <v>0.959071801815046</v>
+        <v>0.754621805503748</v>
       </c>
       <c r="I43" t="n">
-        <v>0.721446736368104</v>
+        <v>0.462126548099792</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>223867120698.016</v>
+        <v>1090.6165331995</v>
       </c>
       <c r="C44" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="D44" t="s">
         <v>17</v>
       </c>
       <c r="E44" t="n">
-        <v>762579127591.92</v>
+        <v>2369.77043627992</v>
       </c>
       <c r="F44" t="n">
-        <v>0.29356575940512</v>
+        <v>0.460220330417976</v>
       </c>
       <c r="G44" t="s">
-        <v>23</v>
+        <v>37</v>
       </c>
       <c r="H44" t="n">
-        <v>0.848663059551276</v>
+        <v>0.689943487481737</v>
       </c>
       <c r="I44" t="n">
-        <v>0.701880179848715</v>
+        <v>0.459833322272749</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B45" t="n">
-        <v>2639496832.16</v>
+        <v>938.298240487</v>
       </c>
       <c r="C45" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="D45" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E45" t="n">
-        <v>6605038847.6</v>
+        <v>1607.191308688</v>
       </c>
       <c r="F45" t="n">
-        <v>0.399618668877184</v>
+        <v>0.583812415743439</v>
       </c>
       <c r="G45" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="H45" t="n">
-        <v>0.731129138076159</v>
+        <v>0.75392522216484</v>
       </c>
       <c r="I45" t="n">
-        <v>0.531319803637567</v>
+        <v>0.46201901429312</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B46" t="n">
-        <v>14238811019.293</v>
+        <v>352380229527.506</v>
       </c>
       <c r="C46" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="D46" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E46" t="n">
-        <v>33711877353.0725</v>
+        <v>1238053003179.45</v>
       </c>
       <c r="F46" t="n">
-        <v>0.422367786586506</v>
+        <v>0.28462451011593</v>
       </c>
       <c r="G46" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="H46" t="n">
-        <v>0.968789564104771</v>
+        <v>0.965411262461457</v>
       </c>
       <c r="I46" t="n">
-        <v>0.757605670811518</v>
+        <v>0.823099007403492</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B47" t="n">
-        <v>3970583353</v>
+        <v>17356975844.8493</v>
       </c>
       <c r="C47" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="D47" t="s">
         <v>20</v>
       </c>
       <c r="E47" t="n">
-        <v>7618629943</v>
+        <v>36521769730.4009</v>
       </c>
       <c r="F47" t="n">
-        <v>0.521167635481255</v>
+        <v>0.475250130893883</v>
       </c>
       <c r="G47" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="H47" t="n">
-        <v>0.828995581916007</v>
+        <v>0.959071801815046</v>
       </c>
       <c r="I47" t="n">
-        <v>0.568411764175379</v>
+        <v>0.721446736368104</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B48" t="n">
-        <v>23200881646.6394</v>
+        <v>223867120698.016</v>
       </c>
       <c r="C48" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="D48" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E48" t="n">
-        <v>51044144755.8797</v>
+        <v>762579127591.92</v>
       </c>
       <c r="F48" t="n">
-        <v>0.454525817948334</v>
+        <v>0.29356575940512</v>
       </c>
       <c r="G48" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="H48" t="n">
-        <v>0.935434979237293</v>
+        <v>0.848663059551276</v>
       </c>
       <c r="I48" t="n">
-        <v>0.708172070263126</v>
+        <v>0.701880179848715</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B49" t="n">
-        <v>25840378478.7994</v>
+        <v>2639496832.16</v>
       </c>
       <c r="C49" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D49" t="s">
         <v>20</v>
       </c>
       <c r="E49" t="n">
-        <v>57649183603.4797</v>
+        <v>6605038847.6</v>
       </c>
       <c r="F49" t="n">
-        <v>0.448234942172531</v>
+        <v>0.399618668877184</v>
       </c>
       <c r="G49" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="H49" t="n">
-        <v>0.912027049873669</v>
+        <v>0.731129138076159</v>
       </c>
       <c r="I49" t="n">
-        <v>0.687909578787403</v>
+        <v>0.531319803637567</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B50" t="n">
-        <v>349.720883370764</v>
+        <v>14522880002.6493</v>
       </c>
       <c r="C50" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="D50" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E50" t="n">
-        <v>1613.7765720005</v>
+        <v>34010118873.7897</v>
       </c>
       <c r="F50" t="n">
-        <v>0.21670960493449</v>
+        <v>0.427016443445647</v>
       </c>
       <c r="G50" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="H50" t="n">
-        <v>0.97130927051774</v>
+        <v>0.969040738820328</v>
       </c>
       <c r="I50" t="n">
-        <v>0.862954468050495</v>
+        <v>0.755532517097505</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B51" t="n">
-        <v>573.58800406878</v>
+        <v>3970583353</v>
       </c>
       <c r="C51" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="D51" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E51" t="n">
-        <v>2371.79921725908</v>
+        <v>7618629943</v>
       </c>
       <c r="F51" t="n">
-        <v>0.241836661339164</v>
+        <v>0.521167635481255</v>
       </c>
       <c r="G51" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="H51" t="n">
-        <v>0.931821033620727</v>
+        <v>0.828995581916007</v>
       </c>
       <c r="I51" t="n">
-        <v>0.810902702951145</v>
+        <v>0.568411764175379</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B52" t="n">
-        <v>42822690385.7787</v>
+        <v>23200881646.6394</v>
       </c>
       <c r="C52" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
       <c r="D52" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E52" t="n">
-        <v>1238053003179.45</v>
+        <v>51044144755.8797</v>
       </c>
       <c r="F52" t="n">
-        <v>0.0345887375385428</v>
+        <v>0.454525817948334</v>
       </c>
       <c r="G52" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H52" t="n">
-        <v>1</v>
+        <v>0.935434979237293</v>
       </c>
       <c r="I52" t="n">
-        <v>0.982705631230729</v>
+        <v>0.708172070263126</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B53" t="n">
-        <v>1494770229.59111</v>
+        <v>25840378478.7994</v>
       </c>
       <c r="C53" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D53" t="s">
         <v>20</v>
       </c>
       <c r="E53" t="n">
-        <v>36521769730.4009</v>
+        <v>57649183603.4797</v>
       </c>
       <c r="F53" t="n">
-        <v>0.0409281981849542</v>
+        <v>0.448234942172531</v>
       </c>
       <c r="G53" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="H53" t="n">
-        <v>1</v>
+        <v>0.912027049873669</v>
       </c>
       <c r="I53" t="n">
-        <v>0.979535900907523</v>
+        <v>0.687909578787403</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B54" t="n">
-        <v>115406392019.819</v>
+        <v>349.226381275</v>
       </c>
       <c r="C54" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="D54" t="s">
         <v>17</v>
       </c>
       <c r="E54" t="n">
-        <v>762579127591.92</v>
+        <v>1611.753827743</v>
       </c>
       <c r="F54" t="n">
-        <v>0.151336940448724</v>
+        <v>0.216674764634519</v>
       </c>
       <c r="G54" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="H54" t="n">
-        <v>1</v>
+        <v>0.971296570138267</v>
       </c>
       <c r="I54" t="n">
-        <v>0.924331529775638</v>
+        <v>0.862959187821008</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B55" t="n">
-        <v>1775902487.99467</v>
+        <v>573.093501973016</v>
       </c>
       <c r="C55" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="D55" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E55" t="n">
-        <v>6605038847.6</v>
+        <v>2369.77043627992</v>
       </c>
       <c r="F55" t="n">
-        <v>0.268870861923841</v>
+        <v>0.241835028912194</v>
       </c>
       <c r="G55" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="H55" t="n">
-        <v>1</v>
+        <v>0.931778516393931</v>
       </c>
       <c r="I55" t="n">
-        <v>0.865564569038079</v>
+        <v>0.810861001937834</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B56" t="n">
-        <v>1052162387.0359</v>
+        <v>349.226381275</v>
       </c>
       <c r="C56" t="s">
-        <v>26</v>
+        <v>38</v>
       </c>
       <c r="D56" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E56" t="n">
-        <v>33711877353.0725</v>
+        <v>1607.191308688</v>
       </c>
       <c r="F56" t="n">
-        <v>0.0312104358952294</v>
+        <v>0.217289864241541</v>
       </c>
       <c r="G56" t="s">
-        <v>27</v>
+        <v>39</v>
       </c>
       <c r="H56" t="n">
-        <v>1</v>
+        <v>0.971215086406381</v>
       </c>
       <c r="I56" t="n">
-        <v>0.984394782052385</v>
+        <v>0.86257015428561</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B57" t="n">
-        <v>1302819380</v>
+        <v>42822690385.7787</v>
       </c>
       <c r="C57" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="D57" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E57" t="n">
-        <v>7618629943</v>
+        <v>1238053003179.45</v>
       </c>
       <c r="F57" t="n">
-        <v>0.171004418083993</v>
+        <v>0.0345887375385428</v>
       </c>
       <c r="G57" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="H57" t="n">
         <v>1</v>
       </c>
       <c r="I57" t="n">
-        <v>0.914497790958003</v>
+        <v>0.982705631230729</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B58" t="n">
-        <v>3295666265.97798</v>
+        <v>1494770229.59111</v>
       </c>
       <c r="C58" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D58" t="s">
         <v>20</v>
       </c>
       <c r="E58" t="n">
-        <v>51044144755.8797</v>
+        <v>36521769730.4009</v>
       </c>
       <c r="F58" t="n">
-        <v>0.0645650207627067</v>
+        <v>0.0409281981849542</v>
       </c>
       <c r="G58" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="H58" t="n">
         <v>1</v>
       </c>
       <c r="I58" t="n">
-        <v>0.967717489618647</v>
+        <v>0.979535900907523</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B59" t="n">
-        <v>5071568753.97265</v>
+        <v>115406392019.819</v>
       </c>
       <c r="C59" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="D59" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E59" t="n">
-        <v>57649183603.4797</v>
+        <v>762579127591.92</v>
       </c>
       <c r="F59" t="n">
-        <v>0.0879729501263315</v>
+        <v>0.151336940448724</v>
       </c>
       <c r="G59" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="H59" t="n">
         <v>1</v>
       </c>
       <c r="I59" t="n">
-        <v>0.956013524936834</v>
+        <v>0.924331529775638</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B60" t="n">
-        <v>46.300427072075</v>
+        <v>1775902487.99467</v>
       </c>
       <c r="C60" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="D60" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E60" t="n">
-        <v>1613.7765720005</v>
+        <v>6605038847.6</v>
       </c>
       <c r="F60" t="n">
-        <v>0.0286907294822599</v>
+        <v>0.268870861923841</v>
       </c>
       <c r="G60" t="s">
-        <v>35</v>
+        <v>25</v>
       </c>
       <c r="H60" t="n">
         <v>1</v>
       </c>
       <c r="I60" t="n">
-        <v>0.98565463525887</v>
+        <v>0.865564569038079</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B61" t="n">
-        <v>161.706819091894</v>
+        <v>1052928152.96533</v>
       </c>
       <c r="C61" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D61" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E61" t="n">
-        <v>2371.79921725908</v>
+        <v>34010118873.7897</v>
       </c>
       <c r="F61" t="n">
-        <v>0.0681789663792732</v>
+        <v>0.0309592611796716</v>
       </c>
       <c r="G61" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="H61" t="n">
         <v>1</v>
       </c>
       <c r="I61" t="n">
-        <v>0.965910516810363</v>
+        <v>0.984520369410164</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>44</v>
+      </c>
+      <c r="B62" t="n">
+        <v>1302819380</v>
+      </c>
+      <c r="C62" t="s">
+        <v>28</v>
+      </c>
+      <c r="D62" t="s">
+        <v>20</v>
+      </c>
+      <c r="E62" t="n">
+        <v>7618629943</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.171004418083993</v>
+      </c>
+      <c r="G62" t="s">
+        <v>29</v>
+      </c>
+      <c r="H62" t="n">
+        <v>1</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.914497790958003</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>44</v>
+      </c>
+      <c r="B63" t="n">
+        <v>3295666265.97798</v>
+      </c>
+      <c r="C63" t="s">
+        <v>30</v>
+      </c>
+      <c r="D63" t="s">
+        <v>20</v>
+      </c>
+      <c r="E63" t="n">
+        <v>51044144755.8797</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.0645650207627067</v>
+      </c>
+      <c r="G63" t="s">
+        <v>31</v>
+      </c>
+      <c r="H63" t="n">
+        <v>1</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.967717489618647</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>44</v>
+      </c>
+      <c r="B64" t="n">
+        <v>5071568753.97265</v>
+      </c>
+      <c r="C64" t="s">
+        <v>32</v>
+      </c>
+      <c r="D64" t="s">
+        <v>20</v>
+      </c>
+      <c r="E64" t="n">
+        <v>57649183603.4797</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.0879729501263315</v>
+      </c>
+      <c r="G64" t="s">
+        <v>33</v>
+      </c>
+      <c r="H64" t="n">
+        <v>1</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.956013524936834</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>44</v>
+      </c>
+      <c r="B65" t="n">
+        <v>46.262862949</v>
+      </c>
+      <c r="C65" t="s">
+        <v>34</v>
+      </c>
+      <c r="D65" t="s">
+        <v>17</v>
+      </c>
+      <c r="E65" t="n">
+        <v>1611.753827743</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.0287034298617324</v>
+      </c>
+      <c r="G65" t="s">
+        <v>35</v>
+      </c>
+      <c r="H65" t="n">
+        <v>1</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.985648285069134</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>44</v>
+      </c>
+      <c r="B66" t="n">
+        <v>161.669254968819</v>
+      </c>
+      <c r="C66" t="s">
+        <v>36</v>
+      </c>
+      <c r="D66" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" t="n">
+        <v>2369.77043627992</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.0682214836060696</v>
+      </c>
+      <c r="G66" t="s">
+        <v>37</v>
+      </c>
+      <c r="H66" t="n">
+        <v>1</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.965889258196965</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>44</v>
+      </c>
+      <c r="B67" t="n">
+        <v>46.262862949</v>
+      </c>
+      <c r="C67" t="s">
+        <v>38</v>
+      </c>
+      <c r="D67" t="s">
+        <v>17</v>
+      </c>
+      <c r="E67" t="n">
+        <v>1607.191308688</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.0287849135936193</v>
+      </c>
+      <c r="G67" t="s">
+        <v>39</v>
+      </c>
+      <c r="H67" t="n">
+        <v>1</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0.98560754320319</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
archiving for IPCC publication
Update all scripts to run on publically available GHG emissions data
Re-organise folders
Remove redundant scripts
</commit_message>
<xml_diff>
--- a/Results/Plot data/ipcc_ar6_figure_equity_perspectives.xlsx
+++ b/Results/Plot data/ipcc_ar6_figure_equity_perspectives.xlsx
@@ -25,7 +25,7 @@
     <t xml:space="preserve">Last update</t>
   </si>
   <si>
-    <t xml:space="preserve">2021-11-05 15:49:12</t>
+    <t xml:space="preserve">2022-02-07 11:57:55</t>
   </si>
   <si>
     <t xml:space="preserve">Code</t>
@@ -902,7 +902,7 @@
         <v>0.136337853751923</v>
       </c>
       <c r="I14" t="n">
-        <v>0.0800840193479043</v>
+        <v>0.0800840193479042</v>
       </c>
     </row>
     <row r="15">
@@ -1096,7 +1096,7 @@
         <v>2410.93684911692</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0894628122165738</v>
+        <v>0.0894628122165739</v>
       </c>
       <c r="G21" t="s">
         <v>29</v>
@@ -1705,7 +1705,7 @@
         <v>2410.93684911692</v>
       </c>
       <c r="F42" t="n">
-        <v>0.0670566112206694</v>
+        <v>0.0670566112206693</v>
       </c>
       <c r="G42" t="s">
         <v>29</v>

</xml_diff>